<commit_message>
Se agrega la clase MiMath con distintas implementaciones de combinatorias y factoriales. También, el triángulo de Tartaglia
</commit_message>
<xml_diff>
--- a/documentacion/Planilla de Métricas V2.1.xlsx
+++ b/documentacion/Planilla de Métricas V2.1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="19440" windowHeight="10170"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Métricas" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="40">
   <si>
     <t>Preparación de la Prueba</t>
   </si>
@@ -119,6 +119,21 @@
   </si>
   <si>
     <t>POLINOMIO</t>
+  </si>
+  <si>
+    <t>Polinomio: atributos y constructores</t>
+  </si>
+  <si>
+    <t>Polinomio: potencias y evaluar</t>
+  </si>
+  <si>
+    <t>Main</t>
+  </si>
+  <si>
+    <t>MiMath: triangulo de Tartaglia</t>
+  </si>
+  <si>
+    <t>MiMath: combinatoria y factoriales</t>
   </si>
 </sst>
 </file>
@@ -824,12 +839,23 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -840,44 +866,23 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="7" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="7" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="2" fontId="2" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -887,32 +892,14 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -923,8 +910,36 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="166" fontId="2" fillId="7" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="7" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -969,7 +984,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="es-ES"/>
+  <c:lang val="es-AR"/>
   <c:chart>
     <c:plotArea>
       <c:layout>
@@ -979,8 +994,8 @@
           <c:yMode val="edge"/>
           <c:x val="3.3565974707706982E-2"/>
           <c:y val="7.4074152627750078E-2"/>
-          <c:w val="0.40158680164979427"/>
-          <c:h val="0.85185169474450073"/>
+          <c:w val="0.40158680164979438"/>
+          <c:h val="0.85185169474450084"/>
         </c:manualLayout>
       </c:layout>
       <c:pieChart>
@@ -1081,10 +1096,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>2.0833333333333333E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>4.2361111111110961E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1101,7 +1116,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.45060916249105226"/>
           <c:y val="0.22139263648838675"/>
-          <c:w val="0.50307062753519516"/>
+          <c:w val="0.50307062753519538"/>
           <c:h val="0.52354412740966338"/>
         </c:manualLayout>
       </c:layout>
@@ -1112,7 +1127,7 @@
           <a:pPr>
             <a:defRPr lang="es-ES"/>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="es-AR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1126,7 +1141,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1454,8 +1469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1"/>
@@ -1470,23 +1485,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="10" customFormat="1" ht="23.25" customHeight="1">
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="62" t="s">
+      <c r="C1" s="92"/>
+      <c r="D1" s="93" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="93"/>
+      <c r="J1" s="93"/>
+      <c r="K1" s="93"/>
+      <c r="L1" s="93"/>
+      <c r="M1" s="93"/>
+      <c r="N1" s="93"/>
     </row>
     <row r="2" spans="1:16" s="10" customFormat="1" ht="5.25" customHeight="1" thickBot="1">
       <c r="B2" s="60"/>
@@ -1505,12 +1520,12 @@
     </row>
     <row r="3" spans="1:16" s="13" customFormat="1" ht="15" customHeight="1">
       <c r="A3" s="11"/>
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="65"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="69"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -1595,12 +1610,12 @@
     </row>
     <row r="7" spans="1:16" s="13" customFormat="1" ht="15" customHeight="1">
       <c r="A7" s="11"/>
-      <c r="B7" s="63" t="s">
+      <c r="B7" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="64"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="65"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="69"/>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
@@ -1626,15 +1641,15 @@
       <c r="E8" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="66"/>
-      <c r="G8" s="66"/>
-      <c r="H8" s="66"/>
-      <c r="I8" s="66"/>
-      <c r="J8" s="66"/>
-      <c r="K8" s="66"/>
-      <c r="L8" s="66"/>
-      <c r="M8" s="66"/>
-      <c r="N8" s="66"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="65"/>
+      <c r="H8" s="65"/>
+      <c r="I8" s="65"/>
+      <c r="J8" s="65"/>
+      <c r="K8" s="65"/>
+      <c r="L8" s="65"/>
+      <c r="M8" s="65"/>
+      <c r="N8" s="65"/>
       <c r="O8" s="14"/>
       <c r="P8" s="18"/>
     </row>
@@ -1653,15 +1668,15 @@
         <f>IFERROR(IF(OR(ISBLANK(C9),ISBLANK(D9)),"Completar",IF(D9&gt;=C9,D9-C9,"Error")),"Error")</f>
         <v>1.9444444444444375E-2</v>
       </c>
-      <c r="F9" s="67"/>
-      <c r="G9" s="67"/>
-      <c r="H9" s="67"/>
-      <c r="I9" s="67"/>
-      <c r="J9" s="67"/>
-      <c r="K9" s="67"/>
-      <c r="L9" s="67"/>
-      <c r="M9" s="67"/>
-      <c r="N9" s="67"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="66"/>
+      <c r="H9" s="66"/>
+      <c r="I9" s="66"/>
+      <c r="J9" s="66"/>
+      <c r="K9" s="66"/>
+      <c r="L9" s="66"/>
+      <c r="M9" s="66"/>
+      <c r="N9" s="66"/>
       <c r="O9" s="19"/>
       <c r="P9" s="22"/>
     </row>
@@ -1685,12 +1700,12 @@
     </row>
     <row r="11" spans="1:16" s="13" customFormat="1" ht="15" customHeight="1">
       <c r="A11" s="11"/>
-      <c r="B11" s="63" t="s">
+      <c r="B11" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="64"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="65"/>
+      <c r="C11" s="68"/>
+      <c r="D11" s="68"/>
+      <c r="E11" s="69"/>
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
@@ -1716,15 +1731,15 @@
       <c r="E12" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="F12" s="66"/>
-      <c r="G12" s="66"/>
-      <c r="H12" s="66"/>
-      <c r="I12" s="66"/>
-      <c r="J12" s="66"/>
-      <c r="K12" s="66"/>
-      <c r="L12" s="66"/>
-      <c r="M12" s="66"/>
-      <c r="N12" s="66"/>
+      <c r="F12" s="65"/>
+      <c r="G12" s="65"/>
+      <c r="H12" s="65"/>
+      <c r="I12" s="65"/>
+      <c r="J12" s="65"/>
+      <c r="K12" s="65"/>
+      <c r="L12" s="65"/>
+      <c r="M12" s="65"/>
+      <c r="N12" s="65"/>
       <c r="O12" s="14"/>
       <c r="P12" s="18"/>
     </row>
@@ -1743,15 +1758,15 @@
         <f>IFERROR(IF(OR(ISBLANK(C13),ISBLANK(D13)),"Completar",IF(D13&gt;=C13,D13-C13,"Error")),"Error")</f>
         <v>4.8611111111112049E-3</v>
       </c>
-      <c r="F13" s="67"/>
-      <c r="G13" s="67"/>
-      <c r="H13" s="67"/>
-      <c r="I13" s="67"/>
-      <c r="J13" s="67"/>
-      <c r="K13" s="67"/>
-      <c r="L13" s="67"/>
-      <c r="M13" s="67"/>
-      <c r="N13" s="67"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="66"/>
+      <c r="H13" s="66"/>
+      <c r="I13" s="66"/>
+      <c r="J13" s="66"/>
+      <c r="K13" s="66"/>
+      <c r="L13" s="66"/>
+      <c r="M13" s="66"/>
+      <c r="N13" s="66"/>
       <c r="O13" s="19"/>
       <c r="P13" s="22"/>
     </row>
@@ -1775,50 +1790,50 @@
     </row>
     <row r="15" spans="1:16" s="13" customFormat="1" ht="15" customHeight="1">
       <c r="A15" s="11"/>
-      <c r="B15" s="63" t="s">
+      <c r="B15" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="64"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="64"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="64"/>
-      <c r="H15" s="64"/>
-      <c r="I15" s="64"/>
-      <c r="J15" s="64"/>
-      <c r="K15" s="64"/>
-      <c r="L15" s="64"/>
-      <c r="M15" s="64"/>
-      <c r="N15" s="65"/>
+      <c r="C15" s="68"/>
+      <c r="D15" s="68"/>
+      <c r="E15" s="68"/>
+      <c r="F15" s="68"/>
+      <c r="G15" s="68"/>
+      <c r="H15" s="68"/>
+      <c r="I15" s="68"/>
+      <c r="J15" s="68"/>
+      <c r="K15" s="68"/>
+      <c r="L15" s="68"/>
+      <c r="M15" s="68"/>
+      <c r="N15" s="69"/>
       <c r="O15" s="11"/>
     </row>
     <row r="16" spans="1:16" s="15" customFormat="1" ht="16.5" customHeight="1">
       <c r="A16" s="14"/>
-      <c r="B16" s="75" t="s">
+      <c r="B16" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="86" t="s">
+      <c r="C16" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="86"/>
-      <c r="E16" s="87"/>
-      <c r="F16" s="88" t="s">
+      <c r="D16" s="74"/>
+      <c r="E16" s="75"/>
+      <c r="F16" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="89"/>
-      <c r="H16" s="85" t="s">
+      <c r="G16" s="62"/>
+      <c r="H16" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="I16" s="86"/>
-      <c r="J16" s="87"/>
-      <c r="K16" s="88" t="s">
+      <c r="I16" s="74"/>
+      <c r="J16" s="75"/>
+      <c r="K16" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="L16" s="89"/>
-      <c r="M16" s="85" t="s">
+      <c r="L16" s="62"/>
+      <c r="M16" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="N16" s="93" t="s">
+      <c r="N16" s="64" t="s">
         <v>2</v>
       </c>
       <c r="O16" s="14"/>
@@ -1826,10 +1841,10 @@
     </row>
     <row r="17" spans="1:16" s="15" customFormat="1" ht="30">
       <c r="A17" s="14"/>
-      <c r="B17" s="75"/>
-      <c r="C17" s="86"/>
-      <c r="D17" s="86"/>
-      <c r="E17" s="87"/>
+      <c r="B17" s="88"/>
+      <c r="C17" s="74"/>
+      <c r="D17" s="74"/>
+      <c r="E17" s="75"/>
       <c r="F17" s="39" t="s">
         <v>12</v>
       </c>
@@ -1851,8 +1866,8 @@
       <c r="L17" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="M17" s="85"/>
-      <c r="N17" s="93"/>
+      <c r="M17" s="63"/>
+      <c r="N17" s="64"/>
       <c r="O17" s="14"/>
       <c r="P17" s="18"/>
     </row>
@@ -1862,23 +1877,39 @@
         <f>ROW($B18)-16</f>
         <v>2</v>
       </c>
-      <c r="C18" s="79"/>
-      <c r="D18" s="79"/>
-      <c r="E18" s="80"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="53" t="str">
+      <c r="C18" s="76" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="76"/>
+      <c r="E18" s="77"/>
+      <c r="F18" s="3">
+        <v>20</v>
+      </c>
+      <c r="G18" s="4">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="H18" s="5">
+        <v>0.88541666666666663</v>
+      </c>
+      <c r="I18" s="6">
+        <v>0.89097222222222217</v>
+      </c>
+      <c r="J18" s="53">
         <f>IFERROR(IF(OR(ISBLANK(H18),ISBLANK(I18)),"",IF(I18&gt;=H18,I18-H18,"Error")),"Error")</f>
-        <v/>
-      </c>
-      <c r="K18" s="7"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="54" t="str">
+        <v>5.5555555555555358E-3</v>
+      </c>
+      <c r="K18" s="7">
+        <v>0</v>
+      </c>
+      <c r="L18" s="8">
+        <v>0</v>
+      </c>
+      <c r="M18" s="9">
+        <v>25</v>
+      </c>
+      <c r="N18" s="54">
         <f>IFERROR(IF(OR(J18="",ISBLANK(L18)),"",J18+L18),"Error")</f>
-        <v/>
+        <v>5.5555555555555358E-3</v>
       </c>
       <c r="O18" s="19"/>
       <c r="P18" s="22"/>
@@ -1889,23 +1920,39 @@
         <f t="shared" ref="B19:B25" si="0">ROW($B19)-16</f>
         <v>3</v>
       </c>
-      <c r="C19" s="79"/>
-      <c r="D19" s="79"/>
-      <c r="E19" s="80"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="53" t="str">
+      <c r="C19" s="76" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="76"/>
+      <c r="E19" s="77"/>
+      <c r="F19" s="3">
+        <v>40</v>
+      </c>
+      <c r="G19" s="4">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="H19" s="5">
+        <v>0.8930555555555556</v>
+      </c>
+      <c r="I19" s="6">
+        <v>0.90833333333333333</v>
+      </c>
+      <c r="J19" s="53">
         <f t="shared" ref="J19:J23" si="1">IFERROR(IF(OR(ISBLANK(H19),ISBLANK(I19)),"",IF(I19&gt;=H19,I19-H19,"Error")),"Error")</f>
-        <v/>
-      </c>
-      <c r="K19" s="7"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="54" t="str">
+        <v>1.5277777777777724E-2</v>
+      </c>
+      <c r="K19" s="7">
+        <v>2</v>
+      </c>
+      <c r="L19" s="8">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="M19" s="9">
+        <v>0</v>
+      </c>
+      <c r="N19" s="54">
         <f t="shared" ref="N19:N25" si="2">IFERROR(IF(OR(J19="",ISBLANK(L19)),"",J19+L19),"Error")</f>
-        <v/>
+        <v>1.6666666666666611E-2</v>
       </c>
       <c r="O19" s="19"/>
       <c r="P19" s="22"/>
@@ -1916,23 +1963,39 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C20" s="79"/>
-      <c r="D20" s="79"/>
-      <c r="E20" s="80"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="53" t="str">
+      <c r="C20" s="76" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="76"/>
+      <c r="E20" s="77"/>
+      <c r="F20" s="3">
+        <v>20</v>
+      </c>
+      <c r="G20" s="4">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="H20" s="5">
+        <v>0.90902777777777777</v>
+      </c>
+      <c r="I20" s="6">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="J20" s="53">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K20" s="7"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="54" t="str">
+        <v>7.6388888888888618E-3</v>
+      </c>
+      <c r="K20" s="7">
+        <v>0</v>
+      </c>
+      <c r="L20" s="8">
+        <v>0</v>
+      </c>
+      <c r="M20" s="9">
+        <v>30</v>
+      </c>
+      <c r="N20" s="54">
         <f t="shared" si="2"/>
-        <v/>
+        <v>7.6388888888888618E-3</v>
       </c>
       <c r="O20" s="19"/>
       <c r="P20" s="22"/>
@@ -1943,23 +2006,39 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C21" s="79"/>
-      <c r="D21" s="79"/>
-      <c r="E21" s="80"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="53" t="str">
+      <c r="C21" s="76" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="76"/>
+      <c r="E21" s="77"/>
+      <c r="F21" s="3">
+        <v>20</v>
+      </c>
+      <c r="G21" s="4">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="H21" s="5">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="I21" s="6">
+        <v>0.92152777777777783</v>
+      </c>
+      <c r="J21" s="53">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K21" s="7"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="54" t="str">
+        <v>4.8611111111112049E-3</v>
+      </c>
+      <c r="K21" s="7">
+        <v>0</v>
+      </c>
+      <c r="L21" s="8">
+        <v>0</v>
+      </c>
+      <c r="M21" s="9">
+        <v>0</v>
+      </c>
+      <c r="N21" s="54">
         <f t="shared" si="2"/>
-        <v/>
+        <v>4.8611111111112049E-3</v>
       </c>
       <c r="O21" s="19"/>
       <c r="P21" s="22"/>
@@ -1970,23 +2049,39 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C22" s="79"/>
-      <c r="D22" s="79"/>
-      <c r="E22" s="80"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="53" t="str">
+      <c r="C22" s="76" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="76"/>
+      <c r="E22" s="77"/>
+      <c r="F22" s="3">
+        <v>20</v>
+      </c>
+      <c r="G22" s="4">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="H22" s="5">
+        <v>0.92152777777777783</v>
+      </c>
+      <c r="I22" s="6">
+        <v>0.93055555555555547</v>
+      </c>
+      <c r="J22" s="53">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K22" s="7"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="54" t="str">
+        <v>9.0277777777776347E-3</v>
+      </c>
+      <c r="K22" s="7">
+        <v>1</v>
+      </c>
+      <c r="L22" s="8">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="M22" s="9">
+        <v>0</v>
+      </c>
+      <c r="N22" s="54">
         <f t="shared" si="2"/>
-        <v/>
+        <v>9.7222222222220784E-3</v>
       </c>
       <c r="O22" s="19"/>
       <c r="P22" s="22"/>
@@ -1997,9 +2092,9 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C23" s="79"/>
-      <c r="D23" s="79"/>
-      <c r="E23" s="80"/>
+      <c r="C23" s="76"/>
+      <c r="D23" s="76"/>
+      <c r="E23" s="77"/>
       <c r="F23" s="3"/>
       <c r="G23" s="4"/>
       <c r="H23" s="5"/>
@@ -2024,9 +2119,9 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C24" s="79"/>
-      <c r="D24" s="79"/>
-      <c r="E24" s="80"/>
+      <c r="C24" s="76"/>
+      <c r="D24" s="76"/>
+      <c r="E24" s="77"/>
       <c r="F24" s="3"/>
       <c r="G24" s="4"/>
       <c r="H24" s="5"/>
@@ -2045,9 +2140,9 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C25" s="79"/>
-      <c r="D25" s="79"/>
-      <c r="E25" s="80"/>
+      <c r="C25" s="76"/>
+      <c r="D25" s="76"/>
+      <c r="E25" s="77"/>
       <c r="F25" s="3"/>
       <c r="G25" s="4"/>
       <c r="H25" s="5"/>
@@ -2068,19 +2163,19 @@
     </row>
     <row r="26" spans="1:16" s="27" customFormat="1" ht="15.75" thickBot="1">
       <c r="A26" s="14"/>
-      <c r="B26" s="90" t="s">
+      <c r="B26" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="91"/>
-      <c r="D26" s="91"/>
-      <c r="E26" s="92"/>
-      <c r="F26" s="45" t="str">
+      <c r="C26" s="82"/>
+      <c r="D26" s="82"/>
+      <c r="E26" s="83"/>
+      <c r="F26" s="45">
         <f>IF(SUM(F18:F25)=0,"Completar",SUM(F18:F25))</f>
-        <v>Completar</v>
-      </c>
-      <c r="G26" s="46" t="str">
+        <v>120</v>
+      </c>
+      <c r="G26" s="46">
         <f>IF(SUM(G18:G25)=0,"Completar",SUM(G18:G25))</f>
-        <v>Completar</v>
+        <v>4.8611111111111112E-2</v>
       </c>
       <c r="H26" s="47" t="s">
         <v>32</v>
@@ -2088,25 +2183,25 @@
       <c r="I26" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="J26" s="49" t="str">
+      <c r="J26" s="49">
         <f>IF(OR(COUNTIF(J18:J25,"Error")&gt;0,COUNTIF(J18:J25,"Completar")&gt;0),"Error",IF(SUM(J18:J25)=0,"Completar",SUM(J18:J25)))</f>
-        <v>Completar</v>
+        <v>4.2361111111110961E-2</v>
       </c>
       <c r="K26" s="50">
         <f>SUM(K18:K25)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L26" s="46">
         <f>SUM(L18:L25)</f>
-        <v>0</v>
-      </c>
-      <c r="M26" s="51" t="str">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="M26" s="51">
         <f>IF(SUM(M18:M25)=0,"Completar",SUM(M18:M25))</f>
-        <v>Completar</v>
-      </c>
-      <c r="N26" s="52" t="str">
+        <v>55</v>
+      </c>
+      <c r="N26" s="52">
         <f>IF(OR(COUNTIF(N18:N25,"Error")&gt;0,COUNTIF(N18:N25,"Completar")&gt;0),"Error",IF(SUM(N18:N25)=0,"Completar",SUM(N18:N25)))</f>
-        <v>Completar</v>
+        <v>4.4444444444444287E-2</v>
       </c>
       <c r="O26" s="14"/>
       <c r="P26" s="26"/>
@@ -2130,12 +2225,12 @@
     </row>
     <row r="28" spans="1:16" s="13" customFormat="1" ht="15" customHeight="1">
       <c r="A28" s="11"/>
-      <c r="B28" s="63" t="s">
+      <c r="B28" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="64"/>
-      <c r="D28" s="64"/>
-      <c r="E28" s="65"/>
+      <c r="C28" s="68"/>
+      <c r="D28" s="68"/>
+      <c r="E28" s="69"/>
       <c r="F28" s="12"/>
       <c r="G28" s="12"/>
       <c r="H28" s="12"/>
@@ -2212,33 +2307,33 @@
       <c r="O31" s="21"/>
     </row>
     <row r="32" spans="1:16">
-      <c r="B32" s="63" t="s">
+      <c r="B32" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="64"/>
-      <c r="D32" s="64"/>
-      <c r="E32" s="64"/>
-      <c r="F32" s="64"/>
-      <c r="G32" s="64"/>
-      <c r="H32" s="64"/>
-      <c r="I32" s="64"/>
-      <c r="J32" s="64"/>
-      <c r="K32" s="64"/>
-      <c r="L32" s="64"/>
-      <c r="M32" s="64"/>
-      <c r="N32" s="65"/>
+      <c r="C32" s="68"/>
+      <c r="D32" s="68"/>
+      <c r="E32" s="68"/>
+      <c r="F32" s="68"/>
+      <c r="G32" s="68"/>
+      <c r="H32" s="68"/>
+      <c r="I32" s="68"/>
+      <c r="J32" s="68"/>
+      <c r="K32" s="68"/>
+      <c r="L32" s="68"/>
+      <c r="M32" s="68"/>
+      <c r="N32" s="69"/>
     </row>
     <row r="33" spans="1:15" ht="15" customHeight="1">
-      <c r="B33" s="70" t="s">
+      <c r="B33" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="71"/>
-      <c r="D33" s="72"/>
-      <c r="E33" s="81" t="str">
+      <c r="C33" s="79"/>
+      <c r="D33" s="80"/>
+      <c r="E33" s="72">
         <f>M26</f>
-        <v>Completar</v>
-      </c>
-      <c r="F33" s="82"/>
+        <v>55</v>
+      </c>
+      <c r="F33" s="73"/>
       <c r="G33" s="29"/>
       <c r="H33" s="30"/>
       <c r="I33" s="30"/>
@@ -2249,16 +2344,16 @@
       <c r="N33" s="31"/>
     </row>
     <row r="34" spans="1:15">
-      <c r="B34" s="70" t="s">
+      <c r="B34" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="71"/>
-      <c r="D34" s="72"/>
-      <c r="E34" s="83" t="str">
+      <c r="C34" s="79"/>
+      <c r="D34" s="80"/>
+      <c r="E34" s="70">
         <f>IF(M26="Completar","Completar",IFERROR(M26/(N26*24),"Error"))</f>
-        <v>Completar</v>
-      </c>
-      <c r="F34" s="84"/>
+        <v>51.562500000000185</v>
+      </c>
+      <c r="F34" s="71"/>
       <c r="G34" s="32"/>
       <c r="H34" s="33"/>
       <c r="I34" s="33"/>
@@ -2269,16 +2364,16 @@
       <c r="N34" s="34"/>
     </row>
     <row r="35" spans="1:15" ht="15" customHeight="1">
-      <c r="B35" s="70" t="s">
+      <c r="B35" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="71"/>
-      <c r="D35" s="72"/>
-      <c r="E35" s="81">
+      <c r="C35" s="79"/>
+      <c r="D35" s="80"/>
+      <c r="E35" s="72">
         <f>IF(K26=0,0,IFERROR(ROUNDUP(K26/(M26/100),0),"Error"))</f>
-        <v>0</v>
-      </c>
-      <c r="F35" s="82"/>
+        <v>6</v>
+      </c>
+      <c r="F35" s="73"/>
       <c r="G35" s="32"/>
       <c r="H35" s="33"/>
       <c r="I35" s="33"/>
@@ -2289,16 +2384,16 @@
       <c r="N35" s="34"/>
     </row>
     <row r="36" spans="1:15" ht="15" customHeight="1">
-      <c r="B36" s="70" t="s">
+      <c r="B36" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="71"/>
-      <c r="D36" s="72"/>
-      <c r="E36" s="68">
+      <c r="C36" s="79"/>
+      <c r="D36" s="80"/>
+      <c r="E36" s="84">
         <f>IF(K26=0,0,IFERROR(K26/M26,"Error"))</f>
-        <v>0</v>
-      </c>
-      <c r="F36" s="69"/>
+        <v>5.4545454545454543E-2</v>
+      </c>
+      <c r="F36" s="85"/>
       <c r="G36" s="32"/>
       <c r="H36" s="33"/>
       <c r="I36" s="33"/>
@@ -2309,18 +2404,18 @@
       <c r="N36" s="34"/>
     </row>
     <row r="37" spans="1:15" ht="15" customHeight="1">
-      <c r="B37" s="70" t="s">
+      <c r="B37" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="C37" s="71"/>
-      <c r="D37" s="72"/>
+      <c r="C37" s="79"/>
+      <c r="D37" s="80"/>
       <c r="E37" s="57">
         <f>E5</f>
         <v>4.8611111111110938E-3</v>
       </c>
       <c r="F37" s="58">
         <f>IF(E37="Completar",E37,IFERROR(E37/$E$43,"Error"))</f>
-        <v>0.16666666666666602</v>
+        <v>6.6037735849056506E-2</v>
       </c>
       <c r="G37" s="32"/>
       <c r="H37" s="33"/>
@@ -2332,18 +2427,18 @@
       <c r="N37" s="34"/>
     </row>
     <row r="38" spans="1:15" ht="15" customHeight="1">
-      <c r="B38" s="70" t="s">
+      <c r="B38" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="C38" s="71"/>
-      <c r="D38" s="72"/>
+      <c r="C38" s="79"/>
+      <c r="D38" s="80"/>
       <c r="E38" s="57">
         <f>E9</f>
         <v>1.9444444444444375E-2</v>
       </c>
       <c r="F38" s="58">
         <f>IF(E38="Completar",E38,IFERROR(E38/$E$43,"Error"))</f>
-        <v>0.66666666666666408</v>
+        <v>0.26415094339622602</v>
       </c>
       <c r="G38" s="32"/>
       <c r="H38" s="33"/>
@@ -2355,18 +2450,18 @@
       <c r="N38" s="34"/>
     </row>
     <row r="39" spans="1:15" ht="15" customHeight="1">
-      <c r="B39" s="70" t="s">
+      <c r="B39" s="78" t="s">
         <v>31</v>
       </c>
-      <c r="C39" s="71"/>
-      <c r="D39" s="72"/>
+      <c r="C39" s="79"/>
+      <c r="D39" s="80"/>
       <c r="E39" s="57">
         <f>E13</f>
         <v>4.8611111111112049E-3</v>
       </c>
       <c r="F39" s="58">
         <f t="shared" ref="F39" si="3">IF(E39="Completar",E39,IFERROR(E39/$E$43,"Error"))</f>
-        <v>0.16666666666666985</v>
+        <v>6.6037735849058019E-2</v>
       </c>
       <c r="G39" s="32"/>
       <c r="H39" s="33"/>
@@ -2378,11 +2473,11 @@
       <c r="N39" s="34"/>
     </row>
     <row r="40" spans="1:15" ht="15" customHeight="1">
-      <c r="B40" s="70" t="s">
+      <c r="B40" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="C40" s="71"/>
-      <c r="D40" s="72"/>
+      <c r="C40" s="79"/>
+      <c r="D40" s="80"/>
       <c r="E40" s="57" t="str">
         <f>E30</f>
         <v>Completar</v>
@@ -2401,18 +2496,18 @@
       <c r="N40" s="34"/>
     </row>
     <row r="41" spans="1:15" ht="15" customHeight="1">
-      <c r="B41" s="70" t="s">
+      <c r="B41" s="78" t="s">
         <v>25</v>
       </c>
-      <c r="C41" s="71"/>
-      <c r="D41" s="72"/>
+      <c r="C41" s="79"/>
+      <c r="D41" s="80"/>
       <c r="E41" s="57">
         <f>L26</f>
-        <v>0</v>
+        <v>2.0833333333333333E-3</v>
       </c>
       <c r="F41" s="58">
         <f>IF(E41="Completar",E41,IFERROR(E41/$E$43,"Completar"))</f>
-        <v>0</v>
+        <v>2.8301886792452886E-2</v>
       </c>
       <c r="G41" s="32"/>
       <c r="H41" s="33"/>
@@ -2424,18 +2519,18 @@
       <c r="N41" s="34"/>
     </row>
     <row r="42" spans="1:15" ht="15" customHeight="1">
-      <c r="B42" s="70" t="s">
+      <c r="B42" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="C42" s="71"/>
-      <c r="D42" s="72"/>
-      <c r="E42" s="57" t="str">
+      <c r="C42" s="79"/>
+      <c r="D42" s="80"/>
+      <c r="E42" s="57">
         <f>J26</f>
-        <v>Completar</v>
-      </c>
-      <c r="F42" s="58" t="str">
+        <v>4.2361111111110961E-2</v>
+      </c>
+      <c r="F42" s="58">
         <f>IF(E42="Completar",E42,IFERROR(E42/$E$43,"Completar"))</f>
-        <v>Completar</v>
+        <v>0.57547169811320664</v>
       </c>
       <c r="G42" s="32"/>
       <c r="H42" s="33"/>
@@ -2447,16 +2542,16 @@
       <c r="N42" s="34"/>
     </row>
     <row r="43" spans="1:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B43" s="76" t="s">
+      <c r="B43" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="C43" s="77"/>
-      <c r="D43" s="78"/>
-      <c r="E43" s="73">
+      <c r="C43" s="90"/>
+      <c r="D43" s="91"/>
+      <c r="E43" s="86">
         <f>IF(COUNTIF(E37:E42,"Error")&gt;0,"Error",IF(SUM(E37:E42)=0,"Completar",SUM(E37:E42)))</f>
-        <v>2.9166666666666674E-2</v>
-      </c>
-      <c r="F43" s="74"/>
+        <v>7.3611111111110961E-2</v>
+      </c>
+      <c r="F43" s="87"/>
       <c r="G43" s="35"/>
       <c r="H43" s="36"/>
       <c r="I43" s="36"/>
@@ -2497,27 +2592,13 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <mergeCells count="44">
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="F8:N8"/>
-    <mergeCell ref="F9:N9"/>
-    <mergeCell ref="B15:N15"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="C16:E17"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:N1"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="F12:N12"/>
+    <mergeCell ref="F13:N13"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B3:E3"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="B42:D42"/>
     <mergeCell ref="E43:F43"/>
@@ -2534,13 +2615,27 @@
     <mergeCell ref="C18:E18"/>
     <mergeCell ref="B39:D39"/>
     <mergeCell ref="E33:F33"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:N1"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="F12:N12"/>
-    <mergeCell ref="F13:N13"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="C16:E17"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="F8:N8"/>
+    <mergeCell ref="F9:N9"/>
+    <mergeCell ref="B15:N15"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:B1048576 D1:XFD1048576 C3:C1048576">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">

</xml_diff>

<commit_message>
Incremento BinomioDeNewton en la planilla de métricas
</commit_message>
<xml_diff>
--- a/documentacion/Planilla de Métricas V2.1.xlsx
+++ b/documentacion/Planilla de Métricas V2.1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
   <si>
     <t>Preparación de la Prueba</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t>MiMath: combinatoria y factoriales</t>
+  </si>
+  <si>
+    <t>BinomioDeNewton: completa</t>
   </si>
 </sst>
 </file>
@@ -647,7 +650,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -839,12 +842,23 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -855,44 +869,23 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="7" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="7" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="2" fontId="2" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -902,32 +895,14 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -938,8 +913,44 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="166" fontId="2" fillId="7" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="7" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -994,8 +1005,8 @@
           <c:yMode val="edge"/>
           <c:x val="3.3565974707706982E-2"/>
           <c:y val="7.4074152627750078E-2"/>
-          <c:w val="0.40158680164979443"/>
-          <c:h val="0.85185169474450095"/>
+          <c:w val="0.40158680164979454"/>
+          <c:h val="0.85185169474450106"/>
         </c:manualLayout>
       </c:layout>
       <c:pieChart>
@@ -1099,7 +1110,7 @@
                   <c:v>2.0833333333333333E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.2361111111110961E-2</c:v>
+                  <c:v>5.2777777777777701E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1116,7 +1127,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.45060916249105226"/>
           <c:y val="0.22139263648838675"/>
-          <c:w val="0.5030706275351956"/>
+          <c:w val="0.50307062753519571"/>
           <c:h val="0.52354412740966338"/>
         </c:manualLayout>
       </c:layout>
@@ -1141,7 +1152,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1470,7 +1481,7 @@
   <dimension ref="A1:P68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="C24" sqref="C24:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1"/>
@@ -1485,23 +1496,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="10" customFormat="1" ht="23.25" customHeight="1">
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="62" t="s">
+      <c r="C1" s="92"/>
+      <c r="D1" s="93" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="93"/>
+      <c r="J1" s="93"/>
+      <c r="K1" s="93"/>
+      <c r="L1" s="93"/>
+      <c r="M1" s="93"/>
+      <c r="N1" s="93"/>
     </row>
     <row r="2" spans="1:16" s="10" customFormat="1" ht="5.25" customHeight="1" thickBot="1">
       <c r="B2" s="60"/>
@@ -1520,12 +1531,12 @@
     </row>
     <row r="3" spans="1:16" s="13" customFormat="1" ht="15" customHeight="1">
       <c r="A3" s="11"/>
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="65"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="69"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -1610,12 +1621,12 @@
     </row>
     <row r="7" spans="1:16" s="13" customFormat="1" ht="15" customHeight="1">
       <c r="A7" s="11"/>
-      <c r="B7" s="63" t="s">
+      <c r="B7" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="64"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="65"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="69"/>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
@@ -1641,15 +1652,15 @@
       <c r="E8" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="66"/>
-      <c r="G8" s="66"/>
-      <c r="H8" s="66"/>
-      <c r="I8" s="66"/>
-      <c r="J8" s="66"/>
-      <c r="K8" s="66"/>
-      <c r="L8" s="66"/>
-      <c r="M8" s="66"/>
-      <c r="N8" s="66"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="65"/>
+      <c r="H8" s="65"/>
+      <c r="I8" s="65"/>
+      <c r="J8" s="65"/>
+      <c r="K8" s="65"/>
+      <c r="L8" s="65"/>
+      <c r="M8" s="65"/>
+      <c r="N8" s="65"/>
       <c r="O8" s="14"/>
       <c r="P8" s="18"/>
     </row>
@@ -1668,15 +1679,15 @@
         <f>IFERROR(IF(OR(ISBLANK(C9),ISBLANK(D9)),"Completar",IF(D9&gt;=C9,D9-C9,"Error")),"Error")</f>
         <v>1.9444444444444375E-2</v>
       </c>
-      <c r="F9" s="67"/>
-      <c r="G9" s="67"/>
-      <c r="H9" s="67"/>
-      <c r="I9" s="67"/>
-      <c r="J9" s="67"/>
-      <c r="K9" s="67"/>
-      <c r="L9" s="67"/>
-      <c r="M9" s="67"/>
-      <c r="N9" s="67"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="66"/>
+      <c r="H9" s="66"/>
+      <c r="I9" s="66"/>
+      <c r="J9" s="66"/>
+      <c r="K9" s="66"/>
+      <c r="L9" s="66"/>
+      <c r="M9" s="66"/>
+      <c r="N9" s="66"/>
       <c r="O9" s="19"/>
       <c r="P9" s="22"/>
     </row>
@@ -1700,12 +1711,12 @@
     </row>
     <row r="11" spans="1:16" s="13" customFormat="1" ht="15" customHeight="1">
       <c r="A11" s="11"/>
-      <c r="B11" s="63" t="s">
+      <c r="B11" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="64"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="65"/>
+      <c r="C11" s="68"/>
+      <c r="D11" s="68"/>
+      <c r="E11" s="69"/>
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
@@ -1731,15 +1742,15 @@
       <c r="E12" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="F12" s="66"/>
-      <c r="G12" s="66"/>
-      <c r="H12" s="66"/>
-      <c r="I12" s="66"/>
-      <c r="J12" s="66"/>
-      <c r="K12" s="66"/>
-      <c r="L12" s="66"/>
-      <c r="M12" s="66"/>
-      <c r="N12" s="66"/>
+      <c r="F12" s="65"/>
+      <c r="G12" s="65"/>
+      <c r="H12" s="65"/>
+      <c r="I12" s="65"/>
+      <c r="J12" s="65"/>
+      <c r="K12" s="65"/>
+      <c r="L12" s="65"/>
+      <c r="M12" s="65"/>
+      <c r="N12" s="65"/>
       <c r="O12" s="14"/>
       <c r="P12" s="18"/>
     </row>
@@ -1758,15 +1769,15 @@
         <f>IFERROR(IF(OR(ISBLANK(C13),ISBLANK(D13)),"Completar",IF(D13&gt;=C13,D13-C13,"Error")),"Error")</f>
         <v>4.8611111111112049E-3</v>
       </c>
-      <c r="F13" s="67"/>
-      <c r="G13" s="67"/>
-      <c r="H13" s="67"/>
-      <c r="I13" s="67"/>
-      <c r="J13" s="67"/>
-      <c r="K13" s="67"/>
-      <c r="L13" s="67"/>
-      <c r="M13" s="67"/>
-      <c r="N13" s="67"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="66"/>
+      <c r="H13" s="66"/>
+      <c r="I13" s="66"/>
+      <c r="J13" s="66"/>
+      <c r="K13" s="66"/>
+      <c r="L13" s="66"/>
+      <c r="M13" s="66"/>
+      <c r="N13" s="66"/>
       <c r="O13" s="19"/>
       <c r="P13" s="22"/>
     </row>
@@ -1790,50 +1801,50 @@
     </row>
     <row r="15" spans="1:16" s="13" customFormat="1" ht="15" customHeight="1">
       <c r="A15" s="11"/>
-      <c r="B15" s="63" t="s">
+      <c r="B15" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="64"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="64"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="64"/>
-      <c r="H15" s="64"/>
-      <c r="I15" s="64"/>
-      <c r="J15" s="64"/>
-      <c r="K15" s="64"/>
-      <c r="L15" s="64"/>
-      <c r="M15" s="64"/>
-      <c r="N15" s="65"/>
+      <c r="C15" s="68"/>
+      <c r="D15" s="68"/>
+      <c r="E15" s="68"/>
+      <c r="F15" s="68"/>
+      <c r="G15" s="68"/>
+      <c r="H15" s="68"/>
+      <c r="I15" s="68"/>
+      <c r="J15" s="68"/>
+      <c r="K15" s="68"/>
+      <c r="L15" s="68"/>
+      <c r="M15" s="68"/>
+      <c r="N15" s="69"/>
       <c r="O15" s="11"/>
     </row>
     <row r="16" spans="1:16" s="15" customFormat="1" ht="16.5" customHeight="1">
       <c r="A16" s="14"/>
-      <c r="B16" s="75" t="s">
+      <c r="B16" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="86" t="s">
+      <c r="C16" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="86"/>
-      <c r="E16" s="87"/>
-      <c r="F16" s="88" t="s">
+      <c r="D16" s="74"/>
+      <c r="E16" s="75"/>
+      <c r="F16" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="89"/>
-      <c r="H16" s="85" t="s">
+      <c r="G16" s="62"/>
+      <c r="H16" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="I16" s="86"/>
-      <c r="J16" s="87"/>
-      <c r="K16" s="88" t="s">
+      <c r="I16" s="74"/>
+      <c r="J16" s="75"/>
+      <c r="K16" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="L16" s="89"/>
-      <c r="M16" s="85" t="s">
+      <c r="L16" s="62"/>
+      <c r="M16" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="N16" s="93" t="s">
+      <c r="N16" s="64" t="s">
         <v>2</v>
       </c>
       <c r="O16" s="14"/>
@@ -1841,10 +1852,10 @@
     </row>
     <row r="17" spans="1:16" s="15" customFormat="1" ht="30">
       <c r="A17" s="14"/>
-      <c r="B17" s="75"/>
-      <c r="C17" s="86"/>
-      <c r="D17" s="86"/>
-      <c r="E17" s="87"/>
+      <c r="B17" s="88"/>
+      <c r="C17" s="74"/>
+      <c r="D17" s="74"/>
+      <c r="E17" s="75"/>
       <c r="F17" s="39" t="s">
         <v>12</v>
       </c>
@@ -1866,8 +1877,8 @@
       <c r="L17" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="M17" s="85"/>
-      <c r="N17" s="93"/>
+      <c r="M17" s="63"/>
+      <c r="N17" s="64"/>
       <c r="O17" s="14"/>
       <c r="P17" s="18"/>
     </row>
@@ -1877,11 +1888,11 @@
         <f>ROW($B18)-16</f>
         <v>2</v>
       </c>
-      <c r="C18" s="79" t="s">
+      <c r="C18" s="76" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="79"/>
-      <c r="E18" s="80"/>
+      <c r="D18" s="76"/>
+      <c r="E18" s="77"/>
       <c r="F18" s="3">
         <v>20</v>
       </c>
@@ -1920,11 +1931,11 @@
         <f t="shared" ref="B19:B25" si="0">ROW($B19)-16</f>
         <v>3</v>
       </c>
-      <c r="C19" s="79" t="s">
+      <c r="C19" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="79"/>
-      <c r="E19" s="80"/>
+      <c r="D19" s="76"/>
+      <c r="E19" s="77"/>
       <c r="F19" s="3">
         <v>40</v>
       </c>
@@ -1963,11 +1974,11 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C20" s="79" t="s">
+      <c r="C20" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="79"/>
-      <c r="E20" s="80"/>
+      <c r="D20" s="76"/>
+      <c r="E20" s="77"/>
       <c r="F20" s="3">
         <v>20</v>
       </c>
@@ -2006,11 +2017,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C21" s="79" t="s">
+      <c r="C21" s="76" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="79"/>
-      <c r="E21" s="80"/>
+      <c r="D21" s="76"/>
+      <c r="E21" s="77"/>
       <c r="F21" s="3">
         <v>20</v>
       </c>
@@ -2049,11 +2060,11 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C22" s="79" t="s">
+      <c r="C22" s="76" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="79"/>
-      <c r="E22" s="80"/>
+      <c r="D22" s="76"/>
+      <c r="E22" s="77"/>
       <c r="F22" s="3">
         <v>20</v>
       </c>
@@ -2092,23 +2103,39 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C23" s="79"/>
-      <c r="D23" s="79"/>
-      <c r="E23" s="80"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="53" t="str">
+      <c r="C23" s="76" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="76"/>
+      <c r="E23" s="77"/>
+      <c r="F23" s="3">
+        <v>50</v>
+      </c>
+      <c r="G23" s="4">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="H23" s="5">
+        <v>0.93055555555555547</v>
+      </c>
+      <c r="I23" s="6">
+        <v>0.94097222222222221</v>
+      </c>
+      <c r="J23" s="53">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K23" s="7"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="54" t="str">
+        <v>1.0416666666666741E-2</v>
+      </c>
+      <c r="K23" s="7">
+        <v>0</v>
+      </c>
+      <c r="L23" s="8">
+        <v>0</v>
+      </c>
+      <c r="M23" s="9">
+        <v>40</v>
+      </c>
+      <c r="N23" s="54">
         <f t="shared" si="2"/>
-        <v/>
+        <v>1.0416666666666741E-2</v>
       </c>
       <c r="O23" s="19"/>
       <c r="P23" s="22"/>
@@ -2119,9 +2146,9 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C24" s="79"/>
-      <c r="D24" s="79"/>
-      <c r="E24" s="80"/>
+      <c r="C24" s="94"/>
+      <c r="D24" s="94"/>
+      <c r="E24" s="95"/>
       <c r="F24" s="3"/>
       <c r="G24" s="4"/>
       <c r="H24" s="5"/>
@@ -2140,9 +2167,9 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C25" s="79"/>
-      <c r="D25" s="79"/>
-      <c r="E25" s="80"/>
+      <c r="C25" s="76"/>
+      <c r="D25" s="76"/>
+      <c r="E25" s="77"/>
       <c r="F25" s="3"/>
       <c r="G25" s="4"/>
       <c r="H25" s="5"/>
@@ -2163,19 +2190,19 @@
     </row>
     <row r="26" spans="1:16" s="27" customFormat="1" ht="15.75" thickBot="1">
       <c r="A26" s="14"/>
-      <c r="B26" s="90" t="s">
+      <c r="B26" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="91"/>
-      <c r="D26" s="91"/>
-      <c r="E26" s="92"/>
+      <c r="C26" s="82"/>
+      <c r="D26" s="82"/>
+      <c r="E26" s="83"/>
       <c r="F26" s="45">
         <f>IF(SUM(F18:F25)=0,"Completar",SUM(F18:F25))</f>
-        <v>120</v>
+        <v>170</v>
       </c>
       <c r="G26" s="46">
         <f>IF(SUM(G18:G25)=0,"Completar",SUM(G18:G25))</f>
-        <v>4.8611111111111112E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="H26" s="47" t="s">
         <v>32</v>
@@ -2185,7 +2212,7 @@
       </c>
       <c r="J26" s="49">
         <f>IF(OR(COUNTIF(J18:J25,"Error")&gt;0,COUNTIF(J18:J25,"Completar")&gt;0),"Error",IF(SUM(J18:J25)=0,"Completar",SUM(J18:J25)))</f>
-        <v>4.2361111111110961E-2</v>
+        <v>5.2777777777777701E-2</v>
       </c>
       <c r="K26" s="50">
         <f>SUM(K18:K25)</f>
@@ -2197,11 +2224,11 @@
       </c>
       <c r="M26" s="51">
         <f>IF(SUM(M18:M25)=0,"Completar",SUM(M18:M25))</f>
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="N26" s="52">
         <f>IF(OR(COUNTIF(N18:N25,"Error")&gt;0,COUNTIF(N18:N25,"Completar")&gt;0),"Error",IF(SUM(N18:N25)=0,"Completar",SUM(N18:N25)))</f>
-        <v>4.4444444444444287E-2</v>
+        <v>5.4861111111111027E-2</v>
       </c>
       <c r="O26" s="14"/>
       <c r="P26" s="26"/>
@@ -2225,12 +2252,12 @@
     </row>
     <row r="28" spans="1:16" s="13" customFormat="1" ht="15" customHeight="1">
       <c r="A28" s="11"/>
-      <c r="B28" s="63" t="s">
+      <c r="B28" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="64"/>
-      <c r="D28" s="64"/>
-      <c r="E28" s="65"/>
+      <c r="C28" s="68"/>
+      <c r="D28" s="68"/>
+      <c r="E28" s="69"/>
       <c r="F28" s="12"/>
       <c r="G28" s="12"/>
       <c r="H28" s="12"/>
@@ -2307,33 +2334,33 @@
       <c r="O31" s="21"/>
     </row>
     <row r="32" spans="1:16">
-      <c r="B32" s="63" t="s">
+      <c r="B32" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="64"/>
-      <c r="D32" s="64"/>
-      <c r="E32" s="64"/>
-      <c r="F32" s="64"/>
-      <c r="G32" s="64"/>
-      <c r="H32" s="64"/>
-      <c r="I32" s="64"/>
-      <c r="J32" s="64"/>
-      <c r="K32" s="64"/>
-      <c r="L32" s="64"/>
-      <c r="M32" s="64"/>
-      <c r="N32" s="65"/>
+      <c r="C32" s="68"/>
+      <c r="D32" s="68"/>
+      <c r="E32" s="68"/>
+      <c r="F32" s="68"/>
+      <c r="G32" s="68"/>
+      <c r="H32" s="68"/>
+      <c r="I32" s="68"/>
+      <c r="J32" s="68"/>
+      <c r="K32" s="68"/>
+      <c r="L32" s="68"/>
+      <c r="M32" s="68"/>
+      <c r="N32" s="69"/>
     </row>
     <row r="33" spans="1:15" ht="15" customHeight="1">
-      <c r="B33" s="70" t="s">
+      <c r="B33" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="71"/>
-      <c r="D33" s="72"/>
-      <c r="E33" s="81">
+      <c r="C33" s="79"/>
+      <c r="D33" s="80"/>
+      <c r="E33" s="72">
         <f>M26</f>
-        <v>55</v>
-      </c>
-      <c r="F33" s="82"/>
+        <v>95</v>
+      </c>
+      <c r="F33" s="73"/>
       <c r="G33" s="29"/>
       <c r="H33" s="30"/>
       <c r="I33" s="30"/>
@@ -2344,16 +2371,16 @@
       <c r="N33" s="31"/>
     </row>
     <row r="34" spans="1:15">
-      <c r="B34" s="70" t="s">
+      <c r="B34" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="71"/>
-      <c r="D34" s="72"/>
-      <c r="E34" s="83">
+      <c r="C34" s="79"/>
+      <c r="D34" s="80"/>
+      <c r="E34" s="70">
         <f>IF(M26="Completar","Completar",IFERROR(M26/(N26*24),"Error"))</f>
-        <v>51.562500000000185</v>
-      </c>
-      <c r="F34" s="84"/>
+        <v>72.151898734177323</v>
+      </c>
+      <c r="F34" s="71"/>
       <c r="G34" s="32"/>
       <c r="H34" s="33"/>
       <c r="I34" s="33"/>
@@ -2364,16 +2391,16 @@
       <c r="N34" s="34"/>
     </row>
     <row r="35" spans="1:15" ht="15" customHeight="1">
-      <c r="B35" s="70" t="s">
+      <c r="B35" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="71"/>
-      <c r="D35" s="72"/>
-      <c r="E35" s="81">
+      <c r="C35" s="79"/>
+      <c r="D35" s="80"/>
+      <c r="E35" s="72">
         <f>IF(K26=0,0,IFERROR(ROUNDUP(K26/(M26/100),0),"Error"))</f>
-        <v>8</v>
-      </c>
-      <c r="F35" s="82"/>
+        <v>5</v>
+      </c>
+      <c r="F35" s="73"/>
       <c r="G35" s="32"/>
       <c r="H35" s="33"/>
       <c r="I35" s="33"/>
@@ -2384,16 +2411,16 @@
       <c r="N35" s="34"/>
     </row>
     <row r="36" spans="1:15" ht="15" customHeight="1">
-      <c r="B36" s="70" t="s">
+      <c r="B36" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="71"/>
-      <c r="D36" s="72"/>
-      <c r="E36" s="68">
+      <c r="C36" s="79"/>
+      <c r="D36" s="80"/>
+      <c r="E36" s="84">
         <f>IF(K26=0,0,IFERROR(K26/M26,"Error"))</f>
-        <v>7.2727272727272724E-2</v>
-      </c>
-      <c r="F36" s="69"/>
+        <v>4.2105263157894736E-2</v>
+      </c>
+      <c r="F36" s="85"/>
       <c r="G36" s="32"/>
       <c r="H36" s="33"/>
       <c r="I36" s="33"/>
@@ -2404,18 +2431,18 @@
       <c r="N36" s="34"/>
     </row>
     <row r="37" spans="1:15" ht="15" customHeight="1">
-      <c r="B37" s="70" t="s">
+      <c r="B37" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="C37" s="71"/>
-      <c r="D37" s="72"/>
+      <c r="C37" s="79"/>
+      <c r="D37" s="80"/>
       <c r="E37" s="57">
         <f>E5</f>
         <v>4.8611111111110938E-3</v>
       </c>
       <c r="F37" s="58">
         <f>IF(E37="Completar",E37,IFERROR(E37/$E$43,"Error"))</f>
-        <v>6.6037735849056506E-2</v>
+        <v>5.7851239669421337E-2</v>
       </c>
       <c r="G37" s="32"/>
       <c r="H37" s="33"/>
@@ -2427,18 +2454,18 @@
       <c r="N37" s="34"/>
     </row>
     <row r="38" spans="1:15" ht="15" customHeight="1">
-      <c r="B38" s="70" t="s">
+      <c r="B38" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="C38" s="71"/>
-      <c r="D38" s="72"/>
+      <c r="C38" s="79"/>
+      <c r="D38" s="80"/>
       <c r="E38" s="57">
         <f>E9</f>
         <v>1.9444444444444375E-2</v>
       </c>
       <c r="F38" s="58">
         <f>IF(E38="Completar",E38,IFERROR(E38/$E$43,"Error"))</f>
-        <v>0.26415094339622602</v>
+        <v>0.23140495867768535</v>
       </c>
       <c r="G38" s="32"/>
       <c r="H38" s="33"/>
@@ -2450,18 +2477,18 @@
       <c r="N38" s="34"/>
     </row>
     <row r="39" spans="1:15" ht="15" customHeight="1">
-      <c r="B39" s="70" t="s">
+      <c r="B39" s="78" t="s">
         <v>31</v>
       </c>
-      <c r="C39" s="71"/>
-      <c r="D39" s="72"/>
+      <c r="C39" s="79"/>
+      <c r="D39" s="80"/>
       <c r="E39" s="57">
         <f>E13</f>
         <v>4.8611111111112049E-3</v>
       </c>
       <c r="F39" s="58">
         <f t="shared" ref="F39" si="3">IF(E39="Completar",E39,IFERROR(E39/$E$43,"Error"))</f>
-        <v>6.6037735849058019E-2</v>
+        <v>5.7851239669422655E-2</v>
       </c>
       <c r="G39" s="32"/>
       <c r="H39" s="33"/>
@@ -2473,11 +2500,11 @@
       <c r="N39" s="34"/>
     </row>
     <row r="40" spans="1:15" ht="15" customHeight="1">
-      <c r="B40" s="70" t="s">
+      <c r="B40" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="C40" s="71"/>
-      <c r="D40" s="72"/>
+      <c r="C40" s="79"/>
+      <c r="D40" s="80"/>
       <c r="E40" s="57" t="str">
         <f>E30</f>
         <v>Completar</v>
@@ -2496,18 +2523,18 @@
       <c r="N40" s="34"/>
     </row>
     <row r="41" spans="1:15" ht="15" customHeight="1">
-      <c r="B41" s="70" t="s">
+      <c r="B41" s="78" t="s">
         <v>25</v>
       </c>
-      <c r="C41" s="71"/>
-      <c r="D41" s="72"/>
+      <c r="C41" s="79"/>
+      <c r="D41" s="80"/>
       <c r="E41" s="57">
         <f>L26</f>
         <v>2.0833333333333333E-3</v>
       </c>
       <c r="F41" s="58">
         <f>IF(E41="Completar",E41,IFERROR(E41/$E$43,"Completar"))</f>
-        <v>2.8301886792452886E-2</v>
+        <v>2.4793388429752088E-2</v>
       </c>
       <c r="G41" s="32"/>
       <c r="H41" s="33"/>
@@ -2519,18 +2546,18 @@
       <c r="N41" s="34"/>
     </row>
     <row r="42" spans="1:15" ht="15" customHeight="1">
-      <c r="B42" s="70" t="s">
+      <c r="B42" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="C42" s="71"/>
-      <c r="D42" s="72"/>
+      <c r="C42" s="79"/>
+      <c r="D42" s="80"/>
       <c r="E42" s="57">
         <f>J26</f>
-        <v>4.2361111111110961E-2</v>
+        <v>5.2777777777777701E-2</v>
       </c>
       <c r="F42" s="58">
         <f>IF(E42="Completar",E42,IFERROR(E42/$E$43,"Completar"))</f>
-        <v>0.57547169811320664</v>
+        <v>0.62809917355371869</v>
       </c>
       <c r="G42" s="32"/>
       <c r="H42" s="33"/>
@@ -2542,16 +2569,16 @@
       <c r="N42" s="34"/>
     </row>
     <row r="43" spans="1:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B43" s="76" t="s">
+      <c r="B43" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="C43" s="77"/>
-      <c r="D43" s="78"/>
-      <c r="E43" s="73">
+      <c r="C43" s="90"/>
+      <c r="D43" s="91"/>
+      <c r="E43" s="86">
         <f>IF(COUNTIF(E37:E42,"Error")&gt;0,"Error",IF(SUM(E37:E42)=0,"Completar",SUM(E37:E42)))</f>
-        <v>7.3611111111110961E-2</v>
-      </c>
-      <c r="F43" s="74"/>
+        <v>8.4027777777777701E-2</v>
+      </c>
+      <c r="F43" s="87"/>
       <c r="G43" s="35"/>
       <c r="H43" s="36"/>
       <c r="I43" s="36"/>
@@ -2592,27 +2619,13 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <mergeCells count="44">
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="F8:N8"/>
-    <mergeCell ref="F9:N9"/>
-    <mergeCell ref="B15:N15"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="C16:E17"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:N1"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="F12:N12"/>
+    <mergeCell ref="F13:N13"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B3:E3"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="B42:D42"/>
     <mergeCell ref="E43:F43"/>
@@ -2629,13 +2642,27 @@
     <mergeCell ref="C18:E18"/>
     <mergeCell ref="B39:D39"/>
     <mergeCell ref="E33:F33"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:N1"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="F12:N12"/>
-    <mergeCell ref="F13:N13"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="C16:E17"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="F8:N8"/>
+    <mergeCell ref="F9:N9"/>
+    <mergeCell ref="B15:N15"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:B1048576 D1:XFD1048576 C3:C1048576">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">

</xml_diff>

<commit_message>
Se actualiza la planilla de métricas con el incremento Tests
</commit_message>
<xml_diff>
--- a/documentacion/Planilla de Métricas V2.1.xlsx
+++ b/documentacion/Planilla de Métricas V2.1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="42">
   <si>
     <t>Preparación de la Prueba</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t>BinomioDeNewton: completa</t>
+  </si>
+  <si>
+    <t>Tests: BinomioDeNewton y MiMath</t>
   </si>
 </sst>
 </file>
@@ -842,23 +845,12 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -869,23 +861,44 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="7" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="7" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -895,54 +908,32 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="7" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="7" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
+    <xf numFmtId="1" fontId="2" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -951,6 +942,18 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1005,8 +1008,8 @@
           <c:yMode val="edge"/>
           <c:x val="3.3565974707706982E-2"/>
           <c:y val="7.4074152627750078E-2"/>
-          <c:w val="0.40158680164979454"/>
-          <c:h val="0.85185169474450106"/>
+          <c:w val="0.40158680164979466"/>
+          <c:h val="0.85185169474450129"/>
         </c:manualLayout>
       </c:layout>
       <c:pieChart>
@@ -1110,7 +1113,7 @@
                   <c:v>2.0833333333333333E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.2777777777777701E-2</c:v>
+                  <c:v>6.25E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1127,7 +1130,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.45060916249105226"/>
           <c:y val="0.22139263648838675"/>
-          <c:w val="0.50307062753519571"/>
+          <c:w val="0.50307062753519582"/>
           <c:h val="0.52354412740966338"/>
         </c:manualLayout>
       </c:layout>
@@ -1152,7 +1155,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1481,7 +1484,7 @@
   <dimension ref="A1:P68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24:E24"/>
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1"/>
@@ -1496,23 +1499,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="10" customFormat="1" ht="23.25" customHeight="1">
-      <c r="B1" s="92" t="s">
+      <c r="B1" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="92"/>
-      <c r="D1" s="93" t="s">
+      <c r="C1" s="61"/>
+      <c r="D1" s="62" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="G1" s="93"/>
-      <c r="H1" s="93"/>
-      <c r="I1" s="93"/>
-      <c r="J1" s="93"/>
-      <c r="K1" s="93"/>
-      <c r="L1" s="93"/>
-      <c r="M1" s="93"/>
-      <c r="N1" s="93"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="62"/>
     </row>
     <row r="2" spans="1:16" s="10" customFormat="1" ht="5.25" customHeight="1" thickBot="1">
       <c r="B2" s="60"/>
@@ -1531,12 +1534,12 @@
     </row>
     <row r="3" spans="1:16" s="13" customFormat="1" ht="15" customHeight="1">
       <c r="A3" s="11"/>
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="69"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="65"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -1621,12 +1624,12 @@
     </row>
     <row r="7" spans="1:16" s="13" customFormat="1" ht="15" customHeight="1">
       <c r="A7" s="11"/>
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="68"/>
-      <c r="D7" s="68"/>
-      <c r="E7" s="69"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="65"/>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
@@ -1652,15 +1655,15 @@
       <c r="E8" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="65"/>
-      <c r="G8" s="65"/>
-      <c r="H8" s="65"/>
-      <c r="I8" s="65"/>
-      <c r="J8" s="65"/>
-      <c r="K8" s="65"/>
-      <c r="L8" s="65"/>
-      <c r="M8" s="65"/>
-      <c r="N8" s="65"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="66"/>
+      <c r="H8" s="66"/>
+      <c r="I8" s="66"/>
+      <c r="J8" s="66"/>
+      <c r="K8" s="66"/>
+      <c r="L8" s="66"/>
+      <c r="M8" s="66"/>
+      <c r="N8" s="66"/>
       <c r="O8" s="14"/>
       <c r="P8" s="18"/>
     </row>
@@ -1679,15 +1682,15 @@
         <f>IFERROR(IF(OR(ISBLANK(C9),ISBLANK(D9)),"Completar",IF(D9&gt;=C9,D9-C9,"Error")),"Error")</f>
         <v>1.9444444444444375E-2</v>
       </c>
-      <c r="F9" s="66"/>
-      <c r="G9" s="66"/>
-      <c r="H9" s="66"/>
-      <c r="I9" s="66"/>
-      <c r="J9" s="66"/>
-      <c r="K9" s="66"/>
-      <c r="L9" s="66"/>
-      <c r="M9" s="66"/>
-      <c r="N9" s="66"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="67"/>
+      <c r="H9" s="67"/>
+      <c r="I9" s="67"/>
+      <c r="J9" s="67"/>
+      <c r="K9" s="67"/>
+      <c r="L9" s="67"/>
+      <c r="M9" s="67"/>
+      <c r="N9" s="67"/>
       <c r="O9" s="19"/>
       <c r="P9" s="22"/>
     </row>
@@ -1711,12 +1714,12 @@
     </row>
     <row r="11" spans="1:16" s="13" customFormat="1" ht="15" customHeight="1">
       <c r="A11" s="11"/>
-      <c r="B11" s="67" t="s">
+      <c r="B11" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="68"/>
-      <c r="D11" s="68"/>
-      <c r="E11" s="69"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="65"/>
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
@@ -1742,15 +1745,15 @@
       <c r="E12" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="F12" s="65"/>
-      <c r="G12" s="65"/>
-      <c r="H12" s="65"/>
-      <c r="I12" s="65"/>
-      <c r="J12" s="65"/>
-      <c r="K12" s="65"/>
-      <c r="L12" s="65"/>
-      <c r="M12" s="65"/>
-      <c r="N12" s="65"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="66"/>
+      <c r="H12" s="66"/>
+      <c r="I12" s="66"/>
+      <c r="J12" s="66"/>
+      <c r="K12" s="66"/>
+      <c r="L12" s="66"/>
+      <c r="M12" s="66"/>
+      <c r="N12" s="66"/>
       <c r="O12" s="14"/>
       <c r="P12" s="18"/>
     </row>
@@ -1769,15 +1772,15 @@
         <f>IFERROR(IF(OR(ISBLANK(C13),ISBLANK(D13)),"Completar",IF(D13&gt;=C13,D13-C13,"Error")),"Error")</f>
         <v>4.8611111111112049E-3</v>
       </c>
-      <c r="F13" s="66"/>
-      <c r="G13" s="66"/>
-      <c r="H13" s="66"/>
-      <c r="I13" s="66"/>
-      <c r="J13" s="66"/>
-      <c r="K13" s="66"/>
-      <c r="L13" s="66"/>
-      <c r="M13" s="66"/>
-      <c r="N13" s="66"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="67"/>
+      <c r="I13" s="67"/>
+      <c r="J13" s="67"/>
+      <c r="K13" s="67"/>
+      <c r="L13" s="67"/>
+      <c r="M13" s="67"/>
+      <c r="N13" s="67"/>
       <c r="O13" s="19"/>
       <c r="P13" s="22"/>
     </row>
@@ -1801,50 +1804,50 @@
     </row>
     <row r="15" spans="1:16" s="13" customFormat="1" ht="15" customHeight="1">
       <c r="A15" s="11"/>
-      <c r="B15" s="67" t="s">
+      <c r="B15" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="68"/>
-      <c r="D15" s="68"/>
-      <c r="E15" s="68"/>
-      <c r="F15" s="68"/>
-      <c r="G15" s="68"/>
-      <c r="H15" s="68"/>
-      <c r="I15" s="68"/>
-      <c r="J15" s="68"/>
-      <c r="K15" s="68"/>
-      <c r="L15" s="68"/>
-      <c r="M15" s="68"/>
-      <c r="N15" s="69"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="64"/>
+      <c r="F15" s="64"/>
+      <c r="G15" s="64"/>
+      <c r="H15" s="64"/>
+      <c r="I15" s="64"/>
+      <c r="J15" s="64"/>
+      <c r="K15" s="64"/>
+      <c r="L15" s="64"/>
+      <c r="M15" s="64"/>
+      <c r="N15" s="65"/>
       <c r="O15" s="11"/>
     </row>
     <row r="16" spans="1:16" s="15" customFormat="1" ht="16.5" customHeight="1">
       <c r="A16" s="14"/>
-      <c r="B16" s="88" t="s">
+      <c r="B16" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="74" t="s">
+      <c r="C16" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="74"/>
-      <c r="E16" s="75"/>
-      <c r="F16" s="61" t="s">
+      <c r="D16" s="86"/>
+      <c r="E16" s="87"/>
+      <c r="F16" s="88" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="62"/>
-      <c r="H16" s="63" t="s">
+      <c r="G16" s="89"/>
+      <c r="H16" s="85" t="s">
         <v>13</v>
       </c>
-      <c r="I16" s="74"/>
-      <c r="J16" s="75"/>
-      <c r="K16" s="61" t="s">
+      <c r="I16" s="86"/>
+      <c r="J16" s="87"/>
+      <c r="K16" s="88" t="s">
         <v>15</v>
       </c>
-      <c r="L16" s="62"/>
-      <c r="M16" s="63" t="s">
+      <c r="L16" s="89"/>
+      <c r="M16" s="85" t="s">
         <v>17</v>
       </c>
-      <c r="N16" s="64" t="s">
+      <c r="N16" s="95" t="s">
         <v>2</v>
       </c>
       <c r="O16" s="14"/>
@@ -1852,10 +1855,10 @@
     </row>
     <row r="17" spans="1:16" s="15" customFormat="1" ht="30">
       <c r="A17" s="14"/>
-      <c r="B17" s="88"/>
-      <c r="C17" s="74"/>
-      <c r="D17" s="74"/>
-      <c r="E17" s="75"/>
+      <c r="B17" s="75"/>
+      <c r="C17" s="86"/>
+      <c r="D17" s="86"/>
+      <c r="E17" s="87"/>
       <c r="F17" s="39" t="s">
         <v>12</v>
       </c>
@@ -1877,8 +1880,8 @@
       <c r="L17" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="M17" s="63"/>
-      <c r="N17" s="64"/>
+      <c r="M17" s="85"/>
+      <c r="N17" s="95"/>
       <c r="O17" s="14"/>
       <c r="P17" s="18"/>
     </row>
@@ -1888,11 +1891,11 @@
         <f>ROW($B18)-16</f>
         <v>2</v>
       </c>
-      <c r="C18" s="76" t="s">
+      <c r="C18" s="79" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="76"/>
-      <c r="E18" s="77"/>
+      <c r="D18" s="79"/>
+      <c r="E18" s="80"/>
       <c r="F18" s="3">
         <v>20</v>
       </c>
@@ -1931,11 +1934,11 @@
         <f t="shared" ref="B19:B25" si="0">ROW($B19)-16</f>
         <v>3</v>
       </c>
-      <c r="C19" s="76" t="s">
+      <c r="C19" s="79" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="76"/>
-      <c r="E19" s="77"/>
+      <c r="D19" s="79"/>
+      <c r="E19" s="80"/>
       <c r="F19" s="3">
         <v>40</v>
       </c>
@@ -1949,7 +1952,7 @@
         <v>0.90833333333333333</v>
       </c>
       <c r="J19" s="53">
-        <f t="shared" ref="J19:J23" si="1">IFERROR(IF(OR(ISBLANK(H19),ISBLANK(I19)),"",IF(I19&gt;=H19,I19-H19,"Error")),"Error")</f>
+        <f t="shared" ref="J19:J24" si="1">IFERROR(IF(OR(ISBLANK(H19),ISBLANK(I19)),"",IF(I19&gt;=H19,I19-H19,"Error")),"Error")</f>
         <v>1.5277777777777724E-2</v>
       </c>
       <c r="K19" s="7">
@@ -1974,11 +1977,11 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C20" s="76" t="s">
+      <c r="C20" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="76"/>
-      <c r="E20" s="77"/>
+      <c r="D20" s="79"/>
+      <c r="E20" s="80"/>
       <c r="F20" s="3">
         <v>20</v>
       </c>
@@ -2017,11 +2020,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C21" s="76" t="s">
+      <c r="C21" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="76"/>
-      <c r="E21" s="77"/>
+      <c r="D21" s="79"/>
+      <c r="E21" s="80"/>
       <c r="F21" s="3">
         <v>20</v>
       </c>
@@ -2060,11 +2063,11 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C22" s="76" t="s">
+      <c r="C22" s="79" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="76"/>
-      <c r="E22" s="77"/>
+      <c r="D22" s="79"/>
+      <c r="E22" s="80"/>
       <c r="F22" s="3">
         <v>20</v>
       </c>
@@ -2103,11 +2106,11 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C23" s="76" t="s">
+      <c r="C23" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="76"/>
-      <c r="E23" s="77"/>
+      <c r="D23" s="79"/>
+      <c r="E23" s="80"/>
       <c r="F23" s="3">
         <v>50</v>
       </c>
@@ -2146,18 +2149,40 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C24" s="94"/>
-      <c r="D24" s="94"/>
-      <c r="E24" s="95"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="53"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="54"/>
+      <c r="C24" s="79" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="90"/>
+      <c r="E24" s="91"/>
+      <c r="F24" s="3">
+        <v>50</v>
+      </c>
+      <c r="G24" s="4">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="H24" s="5">
+        <v>0.94236111111111109</v>
+      </c>
+      <c r="I24" s="6">
+        <v>0.95208333333333339</v>
+      </c>
+      <c r="J24" s="53">
+        <f t="shared" si="1"/>
+        <v>9.7222222222222987E-3</v>
+      </c>
+      <c r="K24" s="7">
+        <v>0</v>
+      </c>
+      <c r="L24" s="8">
+        <v>0</v>
+      </c>
+      <c r="M24" s="9">
+        <v>90</v>
+      </c>
+      <c r="N24" s="54">
+        <f t="shared" si="2"/>
+        <v>9.7222222222222987E-3</v>
+      </c>
       <c r="O24" s="19"/>
       <c r="P24" s="22"/>
     </row>
@@ -2167,9 +2192,9 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C25" s="76"/>
-      <c r="D25" s="76"/>
-      <c r="E25" s="77"/>
+      <c r="C25" s="79"/>
+      <c r="D25" s="79"/>
+      <c r="E25" s="80"/>
       <c r="F25" s="3"/>
       <c r="G25" s="4"/>
       <c r="H25" s="5"/>
@@ -2190,19 +2215,19 @@
     </row>
     <row r="26" spans="1:16" s="27" customFormat="1" ht="15.75" thickBot="1">
       <c r="A26" s="14"/>
-      <c r="B26" s="81" t="s">
+      <c r="B26" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="82"/>
-      <c r="D26" s="82"/>
-      <c r="E26" s="83"/>
+      <c r="C26" s="93"/>
+      <c r="D26" s="93"/>
+      <c r="E26" s="94"/>
       <c r="F26" s="45">
         <f>IF(SUM(F18:F25)=0,"Completar",SUM(F18:F25))</f>
-        <v>170</v>
+        <v>220</v>
       </c>
       <c r="G26" s="46">
         <f>IF(SUM(G18:G25)=0,"Completar",SUM(G18:G25))</f>
-        <v>6.25E-2</v>
+        <v>7.2916666666666671E-2</v>
       </c>
       <c r="H26" s="47" t="s">
         <v>32</v>
@@ -2212,7 +2237,7 @@
       </c>
       <c r="J26" s="49">
         <f>IF(OR(COUNTIF(J18:J25,"Error")&gt;0,COUNTIF(J18:J25,"Completar")&gt;0),"Error",IF(SUM(J18:J25)=0,"Completar",SUM(J18:J25)))</f>
-        <v>5.2777777777777701E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="K26" s="50">
         <f>SUM(K18:K25)</f>
@@ -2224,11 +2249,11 @@
       </c>
       <c r="M26" s="51">
         <f>IF(SUM(M18:M25)=0,"Completar",SUM(M18:M25))</f>
-        <v>95</v>
+        <v>185</v>
       </c>
       <c r="N26" s="52">
         <f>IF(OR(COUNTIF(N18:N25,"Error")&gt;0,COUNTIF(N18:N25,"Completar")&gt;0),"Error",IF(SUM(N18:N25)=0,"Completar",SUM(N18:N25)))</f>
-        <v>5.4861111111111027E-2</v>
+        <v>6.4583333333333326E-2</v>
       </c>
       <c r="O26" s="14"/>
       <c r="P26" s="26"/>
@@ -2252,12 +2277,12 @@
     </row>
     <row r="28" spans="1:16" s="13" customFormat="1" ht="15" customHeight="1">
       <c r="A28" s="11"/>
-      <c r="B28" s="67" t="s">
+      <c r="B28" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="68"/>
-      <c r="D28" s="68"/>
-      <c r="E28" s="69"/>
+      <c r="C28" s="64"/>
+      <c r="D28" s="64"/>
+      <c r="E28" s="65"/>
       <c r="F28" s="12"/>
       <c r="G28" s="12"/>
       <c r="H28" s="12"/>
@@ -2334,33 +2359,33 @@
       <c r="O31" s="21"/>
     </row>
     <row r="32" spans="1:16">
-      <c r="B32" s="67" t="s">
+      <c r="B32" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="68"/>
-      <c r="D32" s="68"/>
-      <c r="E32" s="68"/>
-      <c r="F32" s="68"/>
-      <c r="G32" s="68"/>
-      <c r="H32" s="68"/>
-      <c r="I32" s="68"/>
-      <c r="J32" s="68"/>
-      <c r="K32" s="68"/>
-      <c r="L32" s="68"/>
-      <c r="M32" s="68"/>
-      <c r="N32" s="69"/>
+      <c r="C32" s="64"/>
+      <c r="D32" s="64"/>
+      <c r="E32" s="64"/>
+      <c r="F32" s="64"/>
+      <c r="G32" s="64"/>
+      <c r="H32" s="64"/>
+      <c r="I32" s="64"/>
+      <c r="J32" s="64"/>
+      <c r="K32" s="64"/>
+      <c r="L32" s="64"/>
+      <c r="M32" s="64"/>
+      <c r="N32" s="65"/>
     </row>
     <row r="33" spans="1:15" ht="15" customHeight="1">
-      <c r="B33" s="78" t="s">
+      <c r="B33" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="79"/>
-      <c r="D33" s="80"/>
-      <c r="E33" s="72">
+      <c r="C33" s="71"/>
+      <c r="D33" s="72"/>
+      <c r="E33" s="81">
         <f>M26</f>
-        <v>95</v>
-      </c>
-      <c r="F33" s="73"/>
+        <v>185</v>
+      </c>
+      <c r="F33" s="82"/>
       <c r="G33" s="29"/>
       <c r="H33" s="30"/>
       <c r="I33" s="30"/>
@@ -2371,16 +2396,16 @@
       <c r="N33" s="31"/>
     </row>
     <row r="34" spans="1:15">
-      <c r="B34" s="78" t="s">
+      <c r="B34" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="79"/>
-      <c r="D34" s="80"/>
-      <c r="E34" s="70">
+      <c r="C34" s="71"/>
+      <c r="D34" s="72"/>
+      <c r="E34" s="83">
         <f>IF(M26="Completar","Completar",IFERROR(M26/(N26*24),"Error"))</f>
-        <v>72.151898734177323</v>
-      </c>
-      <c r="F34" s="71"/>
+        <v>119.35483870967744</v>
+      </c>
+      <c r="F34" s="84"/>
       <c r="G34" s="32"/>
       <c r="H34" s="33"/>
       <c r="I34" s="33"/>
@@ -2391,16 +2416,16 @@
       <c r="N34" s="34"/>
     </row>
     <row r="35" spans="1:15" ht="15" customHeight="1">
-      <c r="B35" s="78" t="s">
+      <c r="B35" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="79"/>
-      <c r="D35" s="80"/>
-      <c r="E35" s="72">
+      <c r="C35" s="71"/>
+      <c r="D35" s="72"/>
+      <c r="E35" s="81">
         <f>IF(K26=0,0,IFERROR(ROUNDUP(K26/(M26/100),0),"Error"))</f>
-        <v>5</v>
-      </c>
-      <c r="F35" s="73"/>
+        <v>3</v>
+      </c>
+      <c r="F35" s="82"/>
       <c r="G35" s="32"/>
       <c r="H35" s="33"/>
       <c r="I35" s="33"/>
@@ -2411,16 +2436,16 @@
       <c r="N35" s="34"/>
     </row>
     <row r="36" spans="1:15" ht="15" customHeight="1">
-      <c r="B36" s="78" t="s">
+      <c r="B36" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="79"/>
-      <c r="D36" s="80"/>
-      <c r="E36" s="84">
+      <c r="C36" s="71"/>
+      <c r="D36" s="72"/>
+      <c r="E36" s="68">
         <f>IF(K26=0,0,IFERROR(K26/M26,"Error"))</f>
-        <v>4.2105263157894736E-2</v>
-      </c>
-      <c r="F36" s="85"/>
+        <v>2.1621621621621623E-2</v>
+      </c>
+      <c r="F36" s="69"/>
       <c r="G36" s="32"/>
       <c r="H36" s="33"/>
       <c r="I36" s="33"/>
@@ -2431,18 +2456,18 @@
       <c r="N36" s="34"/>
     </row>
     <row r="37" spans="1:15" ht="15" customHeight="1">
-      <c r="B37" s="78" t="s">
+      <c r="B37" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="C37" s="79"/>
-      <c r="D37" s="80"/>
+      <c r="C37" s="71"/>
+      <c r="D37" s="72"/>
       <c r="E37" s="57">
         <f>E5</f>
         <v>4.8611111111110938E-3</v>
       </c>
       <c r="F37" s="58">
         <f>IF(E37="Completar",E37,IFERROR(E37/$E$43,"Error"))</f>
-        <v>5.7851239669421337E-2</v>
+        <v>5.185185185185167E-2</v>
       </c>
       <c r="G37" s="32"/>
       <c r="H37" s="33"/>
@@ -2454,18 +2479,18 @@
       <c r="N37" s="34"/>
     </row>
     <row r="38" spans="1:15" ht="15" customHeight="1">
-      <c r="B38" s="78" t="s">
+      <c r="B38" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="C38" s="79"/>
-      <c r="D38" s="80"/>
+      <c r="C38" s="71"/>
+      <c r="D38" s="72"/>
       <c r="E38" s="57">
         <f>E9</f>
         <v>1.9444444444444375E-2</v>
       </c>
       <c r="F38" s="58">
         <f>IF(E38="Completar",E38,IFERROR(E38/$E$43,"Error"))</f>
-        <v>0.23140495867768535</v>
+        <v>0.20740740740740668</v>
       </c>
       <c r="G38" s="32"/>
       <c r="H38" s="33"/>
@@ -2477,18 +2502,18 @@
       <c r="N38" s="34"/>
     </row>
     <row r="39" spans="1:15" ht="15" customHeight="1">
-      <c r="B39" s="78" t="s">
+      <c r="B39" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="C39" s="79"/>
-      <c r="D39" s="80"/>
+      <c r="C39" s="71"/>
+      <c r="D39" s="72"/>
       <c r="E39" s="57">
         <f>E13</f>
         <v>4.8611111111112049E-3</v>
       </c>
       <c r="F39" s="58">
         <f t="shared" ref="F39" si="3">IF(E39="Completar",E39,IFERROR(E39/$E$43,"Error"))</f>
-        <v>5.7851239669422655E-2</v>
+        <v>5.185185185185285E-2</v>
       </c>
       <c r="G39" s="32"/>
       <c r="H39" s="33"/>
@@ -2500,11 +2525,11 @@
       <c r="N39" s="34"/>
     </row>
     <row r="40" spans="1:15" ht="15" customHeight="1">
-      <c r="B40" s="78" t="s">
+      <c r="B40" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="C40" s="79"/>
-      <c r="D40" s="80"/>
+      <c r="C40" s="71"/>
+      <c r="D40" s="72"/>
       <c r="E40" s="57" t="str">
         <f>E30</f>
         <v>Completar</v>
@@ -2523,18 +2548,18 @@
       <c r="N40" s="34"/>
     </row>
     <row r="41" spans="1:15" ht="15" customHeight="1">
-      <c r="B41" s="78" t="s">
+      <c r="B41" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="C41" s="79"/>
-      <c r="D41" s="80"/>
+      <c r="C41" s="71"/>
+      <c r="D41" s="72"/>
       <c r="E41" s="57">
         <f>L26</f>
         <v>2.0833333333333333E-3</v>
       </c>
       <c r="F41" s="58">
         <f>IF(E41="Completar",E41,IFERROR(E41/$E$43,"Completar"))</f>
-        <v>2.4793388429752088E-2</v>
+        <v>2.2222222222222223E-2</v>
       </c>
       <c r="G41" s="32"/>
       <c r="H41" s="33"/>
@@ -2546,18 +2571,18 @@
       <c r="N41" s="34"/>
     </row>
     <row r="42" spans="1:15" ht="15" customHeight="1">
-      <c r="B42" s="78" t="s">
+      <c r="B42" s="70" t="s">
         <v>26</v>
       </c>
-      <c r="C42" s="79"/>
-      <c r="D42" s="80"/>
+      <c r="C42" s="71"/>
+      <c r="D42" s="72"/>
       <c r="E42" s="57">
         <f>J26</f>
-        <v>5.2777777777777701E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="F42" s="58">
         <f>IF(E42="Completar",E42,IFERROR(E42/$E$43,"Completar"))</f>
-        <v>0.62809917355371869</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="G42" s="32"/>
       <c r="H42" s="33"/>
@@ -2569,16 +2594,16 @@
       <c r="N42" s="34"/>
     </row>
     <row r="43" spans="1:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B43" s="89" t="s">
+      <c r="B43" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="C43" s="90"/>
-      <c r="D43" s="91"/>
-      <c r="E43" s="86">
+      <c r="C43" s="77"/>
+      <c r="D43" s="78"/>
+      <c r="E43" s="73">
         <f>IF(COUNTIF(E37:E42,"Error")&gt;0,"Error",IF(SUM(E37:E42)=0,"Completar",SUM(E37:E42)))</f>
-        <v>8.4027777777777701E-2</v>
-      </c>
-      <c r="F43" s="87"/>
+        <v>9.375E-2</v>
+      </c>
+      <c r="F43" s="74"/>
       <c r="G43" s="35"/>
       <c r="H43" s="36"/>
       <c r="I43" s="36"/>
@@ -2619,13 +2644,27 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <mergeCells count="44">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:N1"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="F12:N12"/>
-    <mergeCell ref="F13:N13"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="F8:N8"/>
+    <mergeCell ref="F9:N9"/>
+    <mergeCell ref="B15:N15"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="C16:E17"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="B26:E26"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="B42:D42"/>
     <mergeCell ref="E43:F43"/>
@@ -2642,27 +2681,13 @@
     <mergeCell ref="C18:E18"/>
     <mergeCell ref="B39:D39"/>
     <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="C16:E17"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="F8:N8"/>
-    <mergeCell ref="F9:N9"/>
-    <mergeCell ref="B15:N15"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:N1"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="F12:N12"/>
+    <mergeCell ref="F13:N13"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B3:E3"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:B1048576 D1:XFD1048576 C3:C1048576">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">

</xml_diff>